<commit_message>
feat: enable contract view/edit, fix masive upload mapping, add RPC field
</commit_message>
<xml_diff>
--- a/doc/MATRIZ PRESTADORES DE SERVICIOS 2026.xlsx
+++ b/doc/MATRIZ PRESTADORES DE SERVICIOS 2026.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soporte y Desarrollo\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6472A7B-A30A-47BB-ACD2-9B2DDAC0F16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="ENERO 2026" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ENERO 2026'!$A$1:$CA$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="6Hb3xK1MOZaCGgGA8PlIaUqYxUtVBQAX9M4RQy+NR/Q="/>
@@ -241,9 +235,6 @@
     <t>Fecha de aprobación</t>
   </si>
   <si>
-    <t>Feche de Ejejcución</t>
-  </si>
-  <si>
     <t>NÚMERO TELEFÓNICO</t>
   </si>
   <si>
@@ -413,12 +404,15 @@
   </si>
   <si>
     <t>CR 3 A SUR 6 119 BRR PARQUES DE CASTILLA</t>
+  </si>
+  <si>
+    <t>Fecha de Ejecución</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
@@ -1149,15 +1143,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BC1" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1451,90 +1445,90 @@
         <v>69</v>
       </c>
       <c r="BS1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="BT1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BU1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="7" t="s">
+      <c r="BV1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BW1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="BX1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="7" t="s">
+      <c r="BY1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="7" t="s">
+      <c r="CA1" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="CA1" s="18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:79" s="86" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="D2" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="L2" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L2" s="24" t="s">
+      <c r="O2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="M2" s="68" t="s">
+      <c r="R2" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="69" t="s">
         <v>87</v>
-      </c>
-      <c r="N2" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="R2" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="S2" s="69" t="s">
-        <v>88</v>
       </c>
       <c r="T2" s="33"/>
       <c r="U2" s="64">
@@ -1547,69 +1541,69 @@
         <v>67956000</v>
       </c>
       <c r="X2" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y2" s="72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z2" s="64">
         <v>20124</v>
       </c>
       <c r="AA2" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB2" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="AB2" s="73" t="s">
-        <v>117</v>
-      </c>
       <c r="AC2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="AE2" s="64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AF2" s="64"/>
       <c r="AG2" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH2" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI2" s="74" t="s">
         <v>118</v>
-      </c>
-      <c r="AI2" s="74" t="s">
-        <v>119</v>
       </c>
       <c r="AJ2" s="75">
         <v>0</v>
       </c>
       <c r="AK2" s="76"/>
       <c r="AL2" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO2" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="AM2" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN2" s="26" t="s">
+      <c r="AP2" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="AO2" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP2" s="27" t="s">
+      <c r="AQ2" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="AQ2" s="32" t="s">
+      <c r="AR2" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS2" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="AR2" s="28" t="s">
+      <c r="AT2" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="AS2" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="AT2" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="AU2" s="78">
         <f t="shared" ref="AU2" si="0">BC2*BA2</f>
@@ -1618,19 +1612,19 @@
       <c r="AV2" s="79"/>
       <c r="AW2" s="79"/>
       <c r="AX2" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="AZ2" s="64" t="s">
         <v>95</v>
-      </c>
-      <c r="AY2" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="AZ2" s="64" t="s">
-        <v>96</v>
       </c>
       <c r="BA2" s="64">
         <v>6</v>
       </c>
       <c r="BB2" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BC2" s="41">
         <v>5663000</v>
@@ -1638,28 +1632,28 @@
       <c r="BD2" s="64"/>
       <c r="BE2" s="65"/>
       <c r="BF2" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BG2" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BH2" s="33">
         <v>29180813</v>
       </c>
       <c r="BI2" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ2" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="BK2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="BK2" s="20" t="s">
+      <c r="BL2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="BL2" s="20" t="s">
+      <c r="BM2" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="BM2" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="BN2" s="80">
         <v>46025</v>
@@ -1677,13 +1671,13 @@
         <v>3016744172</v>
       </c>
       <c r="BU2" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="BV2" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="BV2" s="85" t="s">
-        <v>127</v>
-      </c>
       <c r="BW2" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BX2" s="64">
         <v>21</v>
@@ -1862,7 +1856,7 @@
       <c r="CA4" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CA2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:CA2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>